<commit_message>
The allowed functionality to calculate mounts was added.
</commit_message>
<xml_diff>
--- a/Mosquito/mosdb2.xlsx
+++ b/Mosquito/mosdb2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Системы" sheetId="10" r:id="rId1"/>
@@ -681,7 +681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -717,7 +717,7 @@
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C25" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>2.61</v>
+        <v>0.59</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -733,7 +733,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.02</v>
+        <v>1.54</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -749,7 +749,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.56</v>
+        <v>1.83</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -765,7 +765,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.55000000000000004</v>
+        <v>1.45</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -781,7 +781,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.65</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -797,7 +797,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.77</v>
+        <v>2.7</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -813,7 +813,7 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.12</v>
+        <v>2.99</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -829,7 +829,7 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.99</v>
+        <v>1.76</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -845,7 +845,7 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.53</v>
+        <v>2.91</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -861,7 +861,7 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.57</v>
+        <v>1.47</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -877,7 +877,7 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.04</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -893,7 +893,7 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.73</v>
+        <v>0.99</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -909,7 +909,7 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -925,7 +925,7 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96</v>
+        <v>2.91</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -941,7 +941,7 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.84</v>
+        <v>1.22</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -957,7 +957,7 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.53</v>
+        <v>2.84</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -973,7 +973,7 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.73</v>
+        <v>1.17</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -989,7 +989,7 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.87</v>
+        <v>1.02</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.37</v>
+        <v>2.44</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="C22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.12</v>
+        <v>2.98</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="C23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.39</v>
+        <v>2.68</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83</v>
+        <v>1.24</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="C25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.35</v>
+        <v>1.04</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1145,7 +1145,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,7 +1830,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C5" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>0.97</v>
+        <v>1.22</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.83</v>
+        <v>0.74</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1872,7 +1872,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.57999999999999996</v>
+        <v>0.82</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1893,7 +1893,7 @@
       </c>
       <c r="C6" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.5</v>
+        <v>2.95</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1926,7 +1926,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1967,7 +1967,7 @@
       </c>
       <c r="C2" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.94</v>
+        <v>0.97</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.18</v>
+        <v>0.61</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2017,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2071,7 +2071,7 @@
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.8</v>
+        <v>2.5</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2123,8 +2123,8 @@
         <v>80</v>
       </c>
       <c r="C2" s="2">
-        <f t="shared" ref="C2:C13" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>2.54</v>
+        <f t="shared" ref="C2:C6" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
+        <v>1.98</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.04</v>
+        <v>1.53</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2154,7 +2154,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A15" si="1">A3+1</f>
+        <f t="shared" ref="A4:A6" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2162,7 +2162,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.54</v>
+        <v>2.58</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.11</v>
+        <v>0.86</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.57</v>
+        <v>2.36</v>
       </c>
       <c r="D6">
         <v>1</v>

</xml_diff>

<commit_message>
The functionality to calculate knobs was added.
</commit_message>
<xml_diff>
--- a/Mosquito/mosdb2.xlsx
+++ b/Mosquito/mosdb2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Системы" sheetId="10" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="85">
   <si>
     <t>Имя</t>
   </si>
@@ -266,9 +266,6 @@
     <t>Держатель металлический белый</t>
   </si>
   <si>
-    <t>крепление поперечины металл</t>
-  </si>
-  <si>
     <t>Крепление поперечины металл (без паза)</t>
   </si>
   <si>
@@ -285,6 +282,9 @@
   </si>
   <si>
     <t>Ручка металлическая коричневая</t>
+  </si>
+  <si>
+    <t>Крепление поперечины металл</t>
   </si>
 </sst>
 </file>
@@ -717,7 +717,7 @@
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C25" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>0.59</v>
+        <v>2.92</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -733,7 +733,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.54</v>
+        <v>1.35</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -749,7 +749,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.83</v>
+        <v>0.8</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -765,7 +765,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.45</v>
+        <v>1.59</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -781,7 +781,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>2.42</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -797,7 +797,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7</v>
+        <v>1.42</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -813,7 +813,7 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.99</v>
+        <v>2.23</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -829,7 +829,7 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.76</v>
+        <v>0.73</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -845,7 +845,7 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.91</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -861,7 +861,7 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.47</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -877,7 +877,7 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>1.42</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -893,7 +893,7 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99</v>
+        <v>1.83</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -909,7 +909,7 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76</v>
+        <v>1.65</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -925,7 +925,7 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.91</v>
+        <v>1.31</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -941,7 +941,7 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.22</v>
+        <v>2.84</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -957,7 +957,7 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.84</v>
+        <v>2.11</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -973,7 +973,7 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.17</v>
+        <v>0.59</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -989,7 +989,7 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79</v>
+        <v>0.53</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.02</v>
+        <v>2.81</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.44</v>
+        <v>1.62</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="C22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.98</v>
+        <v>2.21</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="C23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.68</v>
+        <v>0.81</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.24</v>
+        <v>0.6</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="C25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.04</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1354,21 +1354,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="46.85546875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="4" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
@@ -1381,11 +1381,12 @@
       <c r="D1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1399,7 +1400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1413,7 +1414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1426,11 +1427,11 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1443,11 +1444,11 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
@@ -1830,7 +1831,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C5" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>1.22</v>
+        <v>1.93</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1851,7 +1852,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1872,7 +1873,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82</v>
+        <v>2.38</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1893,7 +1894,7 @@
       </c>
       <c r="C6" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.95</v>
+        <v>0.67</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1967,7 +1968,7 @@
       </c>
       <c r="C2" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>0.97</v>
+        <v>1.23</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1988,7 +1989,7 @@
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>0.61</v>
+        <v>2.87</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2015,20 +2016,20 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="42.28515625" customWidth="1"/>
-    <col min="3" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="3" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
@@ -2042,15 +2043,18 @@
         <v>41</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2">
         <v>0.75</v>
@@ -2058,23 +2062,29 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.5</v>
+        <v>1.24</v>
       </c>
       <c r="D3">
         <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2120,11 +2130,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C6" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>1.98</v>
+        <v>2.59</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2139,11 +2149,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.53</v>
+        <v>1.87</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2158,11 +2168,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.58</v>
+        <v>2.56</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2177,11 +2187,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86</v>
+        <v>2.02</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2196,11 +2206,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.36</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="D6">
         <v>1</v>

</xml_diff>

<commit_message>
The functionality to calculate felt was added
</commit_message>
<xml_diff>
--- a/Mosquito/mosdb2.xlsx
+++ b/Mosquito/mosdb2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Системы" sheetId="10" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="91">
   <si>
     <t>Имя</t>
   </si>
@@ -260,9 +260,6 @@
     <t>Внутренний</t>
   </si>
   <si>
-    <t>Крепление пластик ДПБ/ДПК</t>
-  </si>
-  <si>
     <t>Держатель металлический белый</t>
   </si>
   <si>
@@ -285,6 +282,27 @@
   </si>
   <si>
     <t>Крепление поперечины металл</t>
+  </si>
+  <si>
+    <t>Держатель металлический коричневый</t>
+  </si>
+  <si>
+    <t>Держатель пластиковый коричневый</t>
+  </si>
+  <si>
+    <t>Держатель пластиковый белый</t>
+  </si>
+  <si>
+    <t>Флажки</t>
+  </si>
+  <si>
+    <t>Держатель металлический для 58/60 и 70 систем</t>
+  </si>
+  <si>
+    <t>Фетр</t>
+  </si>
+  <si>
+    <t>Плумжера</t>
   </si>
 </sst>
 </file>
@@ -717,7 +735,7 @@
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C25" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>2.92</v>
+        <v>0.69</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -733,7 +751,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.35</v>
+        <v>0.67</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -749,7 +767,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
+        <v>1.84</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -765,7 +783,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.59</v>
+        <v>1.88</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -781,7 +799,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.42</v>
+        <v>2.23</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -797,7 +815,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.42</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -813,7 +831,7 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.23</v>
+        <v>1.97</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -829,7 +847,7 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.73</v>
+        <v>2.21</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -845,7 +863,7 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1100000000000001</v>
+        <v>0.99</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -861,7 +879,7 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5099999999999998</v>
+        <v>1.8</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -877,7 +895,7 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.42</v>
+        <v>2.5</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -893,7 +911,7 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.83</v>
+        <v>1.77</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -909,7 +927,7 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.65</v>
+        <v>2.12</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -925,7 +943,7 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.31</v>
+        <v>1.83</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -941,7 +959,7 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.84</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -957,7 +975,7 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.11</v>
+        <v>2.5</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -973,7 +991,7 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59</v>
+        <v>1.02</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -989,7 +1007,7 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53</v>
+        <v>2.64</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1005,7 +1023,7 @@
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.81</v>
+        <v>0.97</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1021,7 +1039,7 @@
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.62</v>
+        <v>2.19</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1037,7 +1055,7 @@
       </c>
       <c r="C22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.21</v>
+        <v>1.72</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1053,7 +1071,7 @@
       </c>
       <c r="C23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81</v>
+        <v>2.13</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1069,7 +1087,7 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6</v>
+        <v>2.56</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1084,7 +1102,7 @@
       </c>
       <c r="C25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1499999999999999</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1100,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,6 +1150,17 @@
       </c>
       <c r="C2">
         <v>1.45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1831,7 +1860,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C5" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>1.93</v>
+        <v>1.99</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1852,7 +1881,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4300000000000002</v>
+        <v>2.69</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1873,7 +1902,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.38</v>
+        <v>1.93</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1894,7 +1923,7 @@
       </c>
       <c r="C6" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>0.67</v>
+        <v>1.98</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1924,9 +1953,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -1937,9 +1966,10 @@
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
@@ -1958,17 +1988,20 @@
       <c r="F1" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.23</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1980,16 +2013,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.87</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2001,13 +2034,137 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C14" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
+        <v>2.57</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.96</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.71</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.35</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2018,7 +2175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -2054,7 +2211,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="2">
         <v>0.75</v>
@@ -2074,11 +2231,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.24</v>
+        <v>2.57</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2130,11 +2287,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C6" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>2.59</v>
+        <v>1.64</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2149,11 +2306,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.87</v>
+        <v>1.59</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2168,11 +2325,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.56</v>
+        <v>1.47</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2187,11 +2344,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.02</v>
+        <v>2.66</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2206,11 +2363,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1200000000000001</v>
+        <v>1.34</v>
       </c>
       <c r="D6">
         <v>1</v>

</xml_diff>

<commit_message>
edit excel file, added extra mount elements in form
</commit_message>
<xml_diff>
--- a/Mosquito/mosdb2.xlsx
+++ b/Mosquito/mosdb2.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!Mosquito\Mosquito\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" tabRatio="608" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Системы" sheetId="10" r:id="rId1"/>
@@ -21,16 +16,17 @@
     <sheet name="Крепления" sheetId="8" r:id="rId7"/>
     <sheet name="Кремпления поперечины" sheetId="11" r:id="rId8"/>
     <sheet name="Ручки" sheetId="12" r:id="rId9"/>
-    <sheet name="Дополнительные детали" sheetId="5" r:id="rId10"/>
-    <sheet name="Комплектующие детали" sheetId="13" r:id="rId11"/>
-    <sheet name="Настройки" sheetId="6" r:id="rId12"/>
+    <sheet name="Дополнительные крепления" sheetId="14" r:id="rId10"/>
+    <sheet name="Дополнительные детали" sheetId="5" r:id="rId11"/>
+    <sheet name="Комплектующие детали" sheetId="13" r:id="rId12"/>
+    <sheet name="Настройки" sheetId="6" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="96">
   <si>
     <t>Имя</t>
   </si>
@@ -303,6 +299,21 @@
   </si>
   <si>
     <t>Плумжера</t>
+  </si>
+  <si>
+    <t>Совместимость</t>
+  </si>
+  <si>
+    <t>Не требуется</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7</t>
+  </si>
+  <si>
+    <t>ДМ 58/60 и 70 систем</t>
+  </si>
+  <si>
+    <t>1,2,3,4</t>
   </si>
 </sst>
 </file>
@@ -419,7 +430,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -454,7 +465,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -697,6 +708,94 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -735,7 +834,7 @@
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C25" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>0.69</v>
+        <v>0.53</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -751,7 +850,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67</v>
+        <v>0.81</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -767,7 +866,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.84</v>
+        <v>2.57</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -783,7 +882,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.88</v>
+        <v>1.51</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -799,7 +898,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.23</v>
+        <v>1.66</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -815,7 +914,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.55000000000000004</v>
+        <v>2.76</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -831,7 +930,7 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.97</v>
+        <v>1.94</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -847,7 +946,7 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.21</v>
+        <v>1.34</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -863,7 +962,7 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -879,7 +978,7 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8</v>
+        <v>1.81</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -895,7 +994,7 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5</v>
+        <v>0.79</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -911,7 +1010,7 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.77</v>
+        <v>1.45</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -927,7 +1026,7 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.12</v>
+        <v>2.5</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -943,7 +1042,7 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.83</v>
+        <v>2.42</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -959,7 +1058,7 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.57999999999999996</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -975,7 +1074,7 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -991,7 +1090,7 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.02</v>
+        <v>2.58</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1007,7 +1106,7 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.64</v>
+        <v>2.4</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1023,7 +1122,7 @@
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1039,7 +1138,7 @@
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.19</v>
+        <v>1.48</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1055,7 +1154,7 @@
       </c>
       <c r="C22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.72</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1071,7 +1170,7 @@
       </c>
       <c r="C23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.13</v>
+        <v>2.36</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1087,7 +1186,7 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.56</v>
+        <v>1.24</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1102,7 +1201,7 @@
       </c>
       <c r="C25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>1.89</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1116,7 +1215,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1169,7 +1268,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -1860,7 +1959,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C5" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>1.99</v>
+        <v>0.79</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1881,7 +1980,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.69</v>
+        <v>2.86</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1902,7 +2001,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.93</v>
+        <v>2.19</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1923,7 +2022,7 @@
       </c>
       <c r="C6" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.98</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1955,8 +2054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2001,7 +2100,7 @@
       </c>
       <c r="C2" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.5299999999999998</v>
+        <v>2.48</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2022,7 +2121,7 @@
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.4500000000000002</v>
+        <v>1.8</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2042,8 +2141,8 @@
         <v>85</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" ref="C4:C14" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>2.57</v>
+        <f t="shared" ref="C4:C8" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
+        <v>2.81</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2064,7 +2163,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96</v>
+        <v>0.87</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2085,7 +2184,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2.06</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2106,7 +2205,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.71</v>
+        <v>1.98</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2127,7 +2226,7 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.35</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2235,7 +2334,7 @@
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.57</v>
+        <v>2.7</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2254,7 +2353,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2291,7 +2390,7 @@
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C6" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>1.64</v>
+        <v>2.04</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2310,7 +2409,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.59</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2329,7 +2428,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.47</v>
+        <v>2.78</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2348,7 +2447,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.66</v>
+        <v>2.12</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2367,7 +2466,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.34</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="D6">
         <v>1</v>

</xml_diff>

<commit_message>
The cross profile mount calculation was added.
</commit_message>
<xml_diff>
--- a/Mosquito/mosdb2.xlsx
+++ b/Mosquito/mosdb2.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!Mosquito\Mosquito\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" tabRatio="608" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" tabRatio="608" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Системы" sheetId="10" r:id="rId1"/>
@@ -21,12 +26,12 @@
     <sheet name="Комплектующие детали" sheetId="13" r:id="rId12"/>
     <sheet name="Настройки" sheetId="6" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="97">
   <si>
     <t>Имя</t>
   </si>
@@ -259,9 +264,6 @@
     <t>Держатель металлический белый</t>
   </si>
   <si>
-    <t>Крепление поперечины металл (без паза)</t>
-  </si>
-  <si>
     <t>Ручка пластиковая белая</t>
   </si>
   <si>
@@ -314,6 +316,12 @@
   </si>
   <si>
     <t>1,2,3,4</t>
+  </si>
+  <si>
+    <t>Крепление поперечины пластик (белое)</t>
+  </si>
+  <si>
+    <t>Крепление поперечины пластик (коричневое)</t>
   </si>
 </sst>
 </file>
@@ -430,7 +438,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -465,7 +473,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -710,7 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -745,7 +753,7 @@
         <v>48</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -753,7 +761,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -768,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -776,7 +784,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="2">
         <v>2.1</v>
@@ -791,7 +799,7 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -844,7 +852,7 @@
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C25" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>2.59</v>
+        <v>1.37</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -860,7 +868,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86</v>
+        <v>1.48</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -876,7 +884,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59</v>
+        <v>1.63</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -892,7 +900,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.46</v>
+        <v>2.76</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -908,7 +916,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87</v>
+        <v>1.45</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -924,7 +932,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.27</v>
+        <v>0.77</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -940,7 +948,7 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.83</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -956,7 +964,7 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5499999999999998</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -972,7 +980,7 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2400000000000002</v>
+        <v>2.19</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -988,7 +996,7 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.78</v>
+        <v>0.71</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1004,7 +1012,7 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0099999999999998</v>
+        <v>0.89</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1020,7 +1028,7 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.85</v>
+        <v>1.91</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1036,7 +1044,7 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2400000000000002</v>
+        <v>0.59</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1052,7 +1060,7 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87</v>
+        <v>2.42</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1068,7 +1076,7 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5499999999999998</v>
+        <v>1.68</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1084,7 +1092,7 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.51</v>
+        <v>1.42</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1100,7 +1108,7 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.58</v>
+        <v>2.74</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1116,7 +1124,7 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.42</v>
+        <v>2.92</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1132,7 +1140,7 @@
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.58</v>
+        <v>1.6</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1148,7 +1156,7 @@
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.21</v>
+        <v>0.54</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1164,7 +1172,7 @@
       </c>
       <c r="C22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.61</v>
+        <v>1.17</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1180,7 +1188,7 @@
       </c>
       <c r="C23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4300000000000002</v>
+        <v>2.27</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1196,7 +1204,7 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.39</v>
+        <v>1.02</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1211,7 +1219,7 @@
       </c>
       <c r="C25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.35</v>
+        <v>2.83</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1266,7 +1274,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1969,7 +1977,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C5" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>2.44</v>
+        <v>0.85</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1990,7 +1998,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5299999999999998</v>
+        <v>2.93</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2011,7 +2019,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9</v>
+        <v>1.01</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2032,7 +2040,7 @@
       </c>
       <c r="C6" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.4500000000000002</v>
+        <v>1.33</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2098,7 +2106,7 @@
         <v>48</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2106,11 +2114,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.5499999999999998</v>
+        <v>0.69</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2131,7 +2139,7 @@
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.82</v>
+        <v>1.52</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2148,11 +2156,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" ref="C4:C8" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>2.4</v>
+        <v>1.43</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2169,11 +2177,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.54</v>
+        <v>1.07</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2190,11 +2198,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.72</v>
+        <v>2.34</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2211,11 +2219,11 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.46</v>
+        <v>1.73</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2232,11 +2240,11 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2282,10 +2290,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2320,7 +2328,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2">
         <v>0.75</v>
@@ -2340,16 +2348,32 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="C3" s="2">
-        <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>0.81</v>
+        <v>0.11</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4">
+        <v>0.44</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>2</v>
       </c>
     </row>
@@ -2396,11 +2420,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C6" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>1.87</v>
+        <v>1.81</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2415,11 +2439,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.77</v>
+        <v>1.67</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2434,11 +2458,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9</v>
+        <v>0.54</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2453,11 +2477,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72</v>
+        <v>2.93</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2472,11 +2496,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.86</v>
+        <v>2.27</v>
       </c>
       <c r="D6">
         <v>1</v>

</xml_diff>